<commit_message>
add coloring columns & add borders
</commit_message>
<xml_diff>
--- a/baza.xlsx
+++ b/baza.xlsx
@@ -35,15 +35,81 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E72929"/>
+        <bgColor rgb="00E72929"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EBC5"/>
+        <bgColor rgb="00C6EBC5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FA7070"/>
+        <bgColor rgb="00FA7070"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C4E4FF"/>
+        <bgColor rgb="00C4E4FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008B93FF"/>
+        <bgColor rgb="008B93FF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -51,13 +117,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00FB6D48"/>
+      </left>
+      <right style="thin">
+        <color rgb="00FB6D48"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <bottom style="thick"/>
+    </border>
+    <border>
+      <left style="thick"/>
+      <right style="thick"/>
+      <bottom style="thick"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -430,7 +550,14 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="2.4" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="26" t="n"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -454,62 +581,62 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="26" t="inlineStr">
         <is>
           <t>nazwa</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="inlineStr">
         <is>
           <t>LOT Polish Airlines</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="inlineStr">
         <is>
           <t>Lufthansa</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="17" t="inlineStr">
         <is>
           <t>British Airways</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="17" t="inlineStr">
         <is>
           <t>Emirates</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="17" t="inlineStr">
         <is>
           <t>Delta Air Lines</t>
         </is>
@@ -542,206 +669,215 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="26" t="inlineStr">
         <is>
           <t>data_wylotu</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="26" t="inlineStr">
         <is>
           <t>data_ladowania</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="26" t="inlineStr">
         <is>
           <t>opoznienie</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="26" t="inlineStr">
         <is>
           <t>samolot_id</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="16" t="n">
         <v>81</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="18" t="n">
         <v>45383</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="19" t="n">
         <v>45383</v>
       </c>
-      <c r="E2" t="n">
+      <c r="D2" s="17" t="n"/>
+      <c r="E2" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="16" t="n">
         <v>82</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="18" t="n">
         <v>45384</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="19" t="n">
         <v>45384</v>
       </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="D3" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="16" t="n">
         <v>83</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="18" t="n">
         <v>45385</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="19" t="n">
         <v>45385</v>
       </c>
-      <c r="E4" t="n">
+      <c r="D4" s="17" t="n"/>
+      <c r="E4" s="16" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="16" t="n">
         <v>84</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="18" t="n">
         <v>45386</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="19" t="n">
         <v>45386</v>
       </c>
-      <c r="E5" t="n">
+      <c r="D5" s="17" t="n"/>
+      <c r="E5" s="16" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="16" t="n">
         <v>85</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="18" t="n">
         <v>45387</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="19" t="n">
         <v>45387</v>
       </c>
-      <c r="E6" t="n">
+      <c r="D6" s="17" t="n"/>
+      <c r="E6" s="16" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="16" t="n">
         <v>86</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="18" t="n">
         <v>45388</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="19" t="n">
         <v>45388</v>
       </c>
-      <c r="E7" t="n">
+      <c r="D7" s="17" t="n"/>
+      <c r="E7" s="16" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="16" t="n">
         <v>87</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="18" t="n">
         <v>45389</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="19" t="n">
         <v>45389</v>
       </c>
-      <c r="E8" t="n">
+      <c r="D8" s="17" t="n"/>
+      <c r="E8" s="16" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="16" t="n">
         <v>88</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="18" t="n">
         <v>45390</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="19" t="n">
         <v>45390</v>
       </c>
-      <c r="D9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" t="n">
+      <c r="D9" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="16" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="16" t="n">
         <v>89</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="18" t="n">
         <v>45391</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="19" t="n">
         <v>45391</v>
       </c>
-      <c r="E10" t="n">
+      <c r="D10" s="17" t="n"/>
+      <c r="E10" s="16" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="16" t="n">
         <v>90</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="18" t="n">
         <v>45392</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="19" t="n">
         <v>45392</v>
       </c>
-      <c r="E11" t="n">
+      <c r="D11" s="17" t="n"/>
+      <c r="E11" s="16" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="16" t="n">
         <v>91</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="18" t="n">
         <v>45393</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="19" t="n">
         <v>45393</v>
       </c>
-      <c r="E12" t="n">
+      <c r="D12" s="17" t="n"/>
+      <c r="E12" s="16" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="16" t="n">
         <v>92</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="18" t="n">
         <v>45394</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="19" t="n">
         <v>45394</v>
       </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
+      <c r="D13" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16" t="n">
         <v>11</v>
       </c>
     </row>
@@ -769,82 +905,82 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="26" t="inlineStr">
         <is>
           <t>nazwa</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="inlineStr">
         <is>
           <t>Boeing 737</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="inlineStr">
         <is>
           <t>Airbus A320</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="17" t="inlineStr">
         <is>
           <t>Boeing 787 Dreamliner</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="17" t="inlineStr">
         <is>
           <t>Airbus A380</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="17" t="inlineStr">
         <is>
           <t>Boeing 777</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="17" t="inlineStr">
         <is>
           <t>Embraer E190</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="17" t="inlineStr">
         <is>
           <t>Bombardier CRJ700</t>
         </is>
@@ -878,307 +1014,312 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="26" t="inlineStr">
         <is>
           <t>imie</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="26" t="inlineStr">
         <is>
           <t>nazwisko</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="26" t="inlineStr">
         <is>
           <t>pesel</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="26" t="inlineStr">
         <is>
           <t>telefon</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="26" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="inlineStr">
         <is>
           <t>Jan</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="16" t="inlineStr">
         <is>
           <t>Kowalski</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="17" t="inlineStr">
         <is>
           <t>12345678901</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="16" t="inlineStr">
         <is>
           <t>123456789</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="17" t="inlineStr">
         <is>
           <t>jan.kowalski@example.com</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="inlineStr">
         <is>
           <t>Anna</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="16" t="inlineStr">
         <is>
           <t>Nowak</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="17" t="inlineStr">
         <is>
           <t>23456789012</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="16" t="inlineStr">
         <is>
           <t>234567890</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="17" t="inlineStr">
         <is>
           <t>anna.nowak@example.com</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="17" t="inlineStr">
         <is>
           <t>Kamil</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="16" t="inlineStr">
         <is>
           <t>Wiśniewski</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="D4" s="17" t="n"/>
+      <c r="E4" s="16" t="inlineStr">
         <is>
           <t>345678901</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="17" t="inlineStr">
         <is>
           <t>kamil.wisniewski@example.com</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="17" t="inlineStr">
         <is>
           <t>Karolina</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="16" t="inlineStr">
         <is>
           <t>Lewandowska</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="17" t="inlineStr">
         <is>
           <t>34567890123</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="16" t="inlineStr">
         <is>
           <t>456789012</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="17" t="inlineStr">
         <is>
           <t>karolina.lewandowska@example.com</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="17" t="inlineStr">
         <is>
           <t>Piotr</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="16" t="inlineStr">
         <is>
           <t>Duda</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="D6" s="17" t="n"/>
+      <c r="E6" s="16" t="inlineStr">
         <is>
           <t>567890123</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="17" t="inlineStr">
         <is>
           <t>piotr.duda@example.com</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="17" t="inlineStr">
         <is>
           <t>Magdalena</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="16" t="inlineStr">
         <is>
           <t>Zając</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="17" t="inlineStr">
         <is>
           <t>45678901234</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="E7" s="16" t="n"/>
+      <c r="F7" s="17" t="inlineStr">
         <is>
           <t>magdalena.zajac@example.com</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="17" t="inlineStr">
         <is>
           <t>Krzysztof</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="16" t="inlineStr">
         <is>
           <t>Wójcik</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="17" t="inlineStr">
         <is>
           <t>56789012345</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="16" t="inlineStr">
         <is>
           <t>678901234</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="17" t="inlineStr">
         <is>
           <t>krzysztof.wojcik@example.com</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="17" t="inlineStr">
         <is>
           <t>Aleksandra</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="16" t="inlineStr">
         <is>
           <t>Kaczmarek</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="17" t="inlineStr">
         <is>
           <t>67890123456</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="E9" s="16" t="n"/>
+      <c r="F9" s="17" t="inlineStr">
         <is>
           <t>aleksandra.kaczmarek@example.com</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="17" t="inlineStr">
         <is>
           <t>Marcin</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="16" t="inlineStr">
         <is>
           <t>Wójcik</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="D10" s="17" t="n"/>
+      <c r="E10" s="16" t="inlineStr">
         <is>
           <t>789012345</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="17" t="inlineStr">
         <is>
           <t>marcin.wojcik@example.com</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="17" t="inlineStr">
         <is>
           <t>Monika</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="16" t="inlineStr">
         <is>
           <t>Kowalczyk</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="17" t="inlineStr">
         <is>
           <t>78901234567</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="16" t="inlineStr">
         <is>
           <t>890123456</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="17" t="inlineStr">
         <is>
           <t>monika.kowalczyk@example.com</t>
         </is>
@@ -1212,434 +1353,434 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="26" t="inlineStr">
         <is>
           <t>numer_siedzenia</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="26" t="inlineStr">
         <is>
           <t>dodatkowy_bagaz</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="26" t="inlineStr">
         <is>
           <t>pasazer_id</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="26" t="inlineStr">
         <is>
           <t>numer_lotu</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="26" t="inlineStr">
         <is>
           <t>status_rezerwacji_id</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="16" t="n">
         <v>21</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="17" t="n">
         <v>12</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16" t="n">
         <v>81</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="16" t="n">
         <v>22</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="C3" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="16" t="n">
         <v>82</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="16" t="n">
         <v>23</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="16" t="n">
         <v>83</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="16" t="n">
         <v>24</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="17" t="n">
         <v>20</v>
       </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="C5" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="16" t="n">
         <v>84</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="16" t="n">
         <v>25</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="16" t="n">
         <v>85</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="16" t="n">
         <v>26</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="16" t="n">
         <v>86</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="16" t="n">
         <v>27</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="C8" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="16" t="n">
         <v>87</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="16" t="n">
         <v>28</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="17" t="n">
         <v>18</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="16" t="n">
         <v>88</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="16" t="n">
         <v>29</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="16" t="n">
         <v>89</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="16" t="n">
         <v>30</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="C11" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" s="16" t="n">
         <v>90</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="16" t="n">
         <v>31</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" s="17" t="n">
         <v>11</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
+      <c r="D12" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16" t="n">
         <v>91</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="16" t="n">
         <v>32</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D13" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" t="n">
+      <c r="D13" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="16" t="n">
         <v>92</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="16" t="n">
         <v>33</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" t="n">
+      <c r="C14" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="16" t="n">
         <v>81</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="16" t="n">
         <v>34</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" s="17" t="n">
         <v>16</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" s="16" t="n">
         <v>82</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="16" t="n">
         <v>35</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" s="17" t="n">
         <v>19</v>
       </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" t="n">
+      <c r="C16" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" s="16" t="n">
         <v>83</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="16" t="n">
         <v>36</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" s="17" t="n">
         <v>13</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" s="16" t="n">
         <v>84</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="16" t="n">
         <v>37</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
-      <c r="D18" t="n">
+      <c r="C18" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" s="16" t="n">
         <v>85</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n">
+      <c r="A19" s="16" t="n">
         <v>38</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" s="17" t="n">
         <v>17</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" s="16" t="n">
         <v>86</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19" s="17" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n">
+      <c r="A20" s="16" t="n">
         <v>39</v>
       </c>
-      <c r="B20" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" t="n">
+      <c r="B20" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" s="16" t="n">
         <v>87</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20" s="17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n">
+      <c r="A21" s="16" t="n">
         <v>40</v>
       </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" t="n">
+      <c r="B21" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" s="16" t="n">
         <v>88</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21" s="17" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1668,140 +1809,140 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="26" t="inlineStr">
         <is>
           <t>linie_lotnicze_id</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="26" t="inlineStr">
         <is>
           <t>model_id</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="A2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="A3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="16" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="16" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="16" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="16" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="16" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="16" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="16" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1829,42 +1970,42 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="26" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="26" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="inlineStr">
         <is>
           <t>Zarezerwowane</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="inlineStr">
         <is>
           <t>Potwierdzone</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="17" t="inlineStr">
         <is>
           <t>Anulowane</t>
         </is>

</xml_diff>